<commit_message>
Fixed removal date of PINT MY busdox; TICC-386
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.2.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philip/dev/git-peppol/edec-codelists/work-in-progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3377576D-3860-B546-B99A-3FF8A5934753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C550A4C-B780-3541-8C30-4800C5EBCF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="839">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2438,13 +2438,6 @@
     <t>Deprecation release / per</t>
   </si>
   <si>
-    <t>deprecation-scheduled</t>
-  </si>
-  <si>
-    <t>TICC-328
-TICC-374</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#conformant#urn:peppol:eb2b:1.0::2.1</t>
   </si>
   <si>
@@ -2636,6 +2629,11 @@
   </si>
   <si>
     <t>cenbii-procid-ubl::urn:peppol:edec:mls</t>
+  </si>
+  <si>
+    <t>TICC-328
+TICC-374
+TICC-386</t>
   </si>
 </sst>
 </file>
@@ -2715,7 +2713,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2731,12 +2729,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2765,7 +2757,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2889,25 +2881,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -3327,8 +3300,8 @@
   <dimension ref="A1:N304"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A304" sqref="A304"/>
+      <pane ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A250" sqref="A250:A253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6154,11 +6127,11 @@
         <v>349</v>
       </c>
       <c r="F72" s="40" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="G72" s="41"/>
       <c r="H72" s="36" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="I72" s="36" t="b">
         <v>0</v>
@@ -6197,11 +6170,11 @@
         <v>349</v>
       </c>
       <c r="F73" s="40" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="G73" s="41"/>
       <c r="H73" s="36" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="I73" s="36" t="b">
         <v>0</v>
@@ -6240,11 +6213,11 @@
         <v>349</v>
       </c>
       <c r="F74" s="40" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="G74" s="41"/>
       <c r="H74" s="36" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="I74" s="36" t="b">
         <v>0</v>
@@ -6281,11 +6254,11 @@
         <v>349</v>
       </c>
       <c r="F75" s="40" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="G75" s="41"/>
       <c r="H75" s="36" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="I75" s="36" t="b">
         <v>0</v>
@@ -12082,7 +12055,7 @@
       <c r="E230" s="24" t="s">
         <v>480</v>
       </c>
-      <c r="F230" s="52" t="s">
+      <c r="F230" s="45" t="s">
         <v>738</v>
       </c>
       <c r="G230" s="18">
@@ -12126,7 +12099,7 @@
       <c r="E231" s="24" t="s">
         <v>480</v>
       </c>
-      <c r="F231" s="52" t="s">
+      <c r="F231" s="45" t="s">
         <v>738</v>
       </c>
       <c r="G231" s="18">
@@ -12170,7 +12143,7 @@
       <c r="E232" s="24" t="s">
         <v>480</v>
       </c>
-      <c r="F232" s="52" t="s">
+      <c r="F232" s="45" t="s">
         <v>738</v>
       </c>
       <c r="G232" s="18">
@@ -12214,7 +12187,7 @@
       <c r="E233" s="24" t="s">
         <v>480</v>
       </c>
-      <c r="F233" s="52" t="s">
+      <c r="F233" s="45" t="s">
         <v>738</v>
       </c>
       <c r="G233" s="18">
@@ -12832,179 +12805,179 @@
         <v>505</v>
       </c>
     </row>
-    <row r="250" spans="1:14" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A250" s="48" t="s">
+    <row r="250" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A250" s="36" t="s">
         <v>631</v>
       </c>
-      <c r="B250" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="C250" s="50" t="s">
+      <c r="B250" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C250" s="36" t="s">
         <v>635</v>
       </c>
-      <c r="D250" s="51" t="s">
+      <c r="D250" s="37" t="s">
         <v>629</v>
       </c>
-      <c r="E250" s="46" t="s">
-        <v>777</v>
-      </c>
-      <c r="F250" s="47">
+      <c r="E250" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="F250" s="35">
         <v>45792</v>
       </c>
-      <c r="G250" s="47">
-        <v>45817</v>
-      </c>
-      <c r="H250" s="45" t="s">
-        <v>778</v>
-      </c>
-      <c r="I250" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J250" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K250" s="46">
+      <c r="G250" s="35">
+        <v>45909</v>
+      </c>
+      <c r="H250" s="36" t="s">
+        <v>838</v>
+      </c>
+      <c r="I250" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J250" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K250" s="33">
         <v>3</v>
       </c>
-      <c r="L250" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="M250" s="46" t="s">
+      <c r="L250" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M250" s="33" t="s">
         <v>691</v>
       </c>
-      <c r="N250" s="45" t="s">
+      <c r="N250" s="36" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="251" spans="1:14" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A251" s="48" t="s">
+    <row r="251" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A251" s="36" t="s">
         <v>632</v>
       </c>
-      <c r="B251" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="C251" s="50" t="s">
+      <c r="B251" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C251" s="36" t="s">
         <v>636</v>
       </c>
-      <c r="D251" s="51" t="s">
+      <c r="D251" s="37" t="s">
         <v>629</v>
       </c>
-      <c r="E251" s="46" t="s">
-        <v>777</v>
-      </c>
-      <c r="F251" s="47">
+      <c r="E251" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="F251" s="35">
         <v>45792</v>
       </c>
-      <c r="G251" s="47">
-        <v>45817</v>
-      </c>
-      <c r="H251" s="45" t="s">
-        <v>778</v>
-      </c>
-      <c r="I251" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J251" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K251" s="46">
+      <c r="G251" s="35">
+        <v>45909</v>
+      </c>
+      <c r="H251" s="36" t="s">
+        <v>838</v>
+      </c>
+      <c r="I251" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J251" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K251" s="33">
         <v>3</v>
       </c>
-      <c r="L251" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="M251" s="46" t="s">
+      <c r="L251" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M251" s="33" t="s">
         <v>692</v>
       </c>
-      <c r="N251" s="45" t="s">
+      <c r="N251" s="36" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="252" spans="1:14" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A252" s="48" t="s">
+    <row r="252" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A252" s="36" t="s">
         <v>633</v>
       </c>
-      <c r="B252" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="C252" s="50" t="s">
+      <c r="B252" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C252" s="36" t="s">
         <v>637</v>
       </c>
-      <c r="D252" s="51" t="s">
+      <c r="D252" s="37" t="s">
         <v>629</v>
       </c>
-      <c r="E252" s="46" t="s">
-        <v>777</v>
-      </c>
-      <c r="F252" s="47">
+      <c r="E252" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="F252" s="35">
         <v>45792</v>
       </c>
-      <c r="G252" s="47">
-        <v>45817</v>
-      </c>
-      <c r="H252" s="45" t="s">
-        <v>778</v>
-      </c>
-      <c r="I252" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J252" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K252" s="46">
+      <c r="G252" s="35">
+        <v>45909</v>
+      </c>
+      <c r="H252" s="36" t="s">
+        <v>838</v>
+      </c>
+      <c r="I252" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J252" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K252" s="33">
         <v>3</v>
       </c>
-      <c r="L252" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="M252" s="46" t="s">
+      <c r="L252" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M252" s="33" t="s">
         <v>691</v>
       </c>
-      <c r="N252" s="45" t="s">
+      <c r="N252" s="36" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="253" spans="1:14" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A253" s="48" t="s">
+    <row r="253" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A253" s="36" t="s">
         <v>634</v>
       </c>
-      <c r="B253" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="C253" s="50" t="s">
+      <c r="B253" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C253" s="36" t="s">
         <v>638</v>
       </c>
-      <c r="D253" s="51" t="s">
+      <c r="D253" s="37" t="s">
         <v>629</v>
       </c>
-      <c r="E253" s="46" t="s">
-        <v>777</v>
-      </c>
-      <c r="F253" s="47">
+      <c r="E253" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="F253" s="35">
         <v>45792</v>
       </c>
-      <c r="G253" s="47">
-        <v>45817</v>
-      </c>
-      <c r="H253" s="45" t="s">
-        <v>778</v>
-      </c>
-      <c r="I253" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J253" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K253" s="46">
+      <c r="G253" s="35">
+        <v>45909</v>
+      </c>
+      <c r="H253" s="36" t="s">
+        <v>838</v>
+      </c>
+      <c r="I253" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J253" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K253" s="33">
         <v>3</v>
       </c>
-      <c r="L253" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="M253" s="46" t="s">
+      <c r="L253" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M253" s="33" t="s">
         <v>692</v>
       </c>
-      <c r="N253" s="45" t="s">
+      <c r="N253" s="36" t="s">
         <v>505</v>
       </c>
     </row>
@@ -14116,13 +14089,13 @@
     </row>
     <row r="284" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="B284" s="5" t="s">
         <v>586</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D284" s="28" t="s">
         <v>738</v>
@@ -14144,21 +14117,21 @@
         <v>111</v>
       </c>
       <c r="M284" s="23" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="N284" s="5" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="285" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B285" s="5" t="s">
         <v>586</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="D285" s="28" t="s">
         <v>738</v>
@@ -14180,21 +14153,21 @@
         <v>111</v>
       </c>
       <c r="M285" s="23" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="N285" s="5" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="286" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A286" s="5" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="B286" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D286" s="28" t="s">
         <v>738</v>
@@ -14203,7 +14176,7 @@
         <v>350</v>
       </c>
       <c r="H286" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I286" s="5" t="b">
         <v>0</v>
@@ -14213,24 +14186,24 @@
         <v>1</v>
       </c>
       <c r="L286" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M286" s="23" t="s">
         <v>691</v>
       </c>
       <c r="N286" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="287" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A287" s="5" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B287" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C287" s="5" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D287" s="28" t="s">
         <v>738</v>
@@ -14239,7 +14212,7 @@
         <v>350</v>
       </c>
       <c r="H287" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I287" s="5" t="b">
         <v>0</v>
@@ -14249,24 +14222,24 @@
         <v>1</v>
       </c>
       <c r="L287" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M287" s="23" t="s">
         <v>692</v>
       </c>
       <c r="N287" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="288" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A288" s="5" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B288" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D288" s="28" t="s">
         <v>738</v>
@@ -14275,7 +14248,7 @@
         <v>350</v>
       </c>
       <c r="H288" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I288" s="5" t="b">
         <v>0</v>
@@ -14285,24 +14258,24 @@
         <v>1</v>
       </c>
       <c r="L288" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M288" s="23" t="s">
         <v>690</v>
       </c>
       <c r="N288" s="5" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="289" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A289" s="5" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B289" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C289" s="5" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D289" s="28" t="s">
         <v>738</v>
@@ -14311,7 +14284,7 @@
         <v>350</v>
       </c>
       <c r="H289" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I289" s="5" t="b">
         <v>0</v>
@@ -14321,24 +14294,24 @@
         <v>1</v>
       </c>
       <c r="L289" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M289" s="23" t="s">
         <v>693</v>
       </c>
       <c r="N289" s="5" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="290" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A290" s="5" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B290" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C290" s="5" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="D290" s="28" t="s">
         <v>738</v>
@@ -14347,7 +14320,7 @@
         <v>350</v>
       </c>
       <c r="H290" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I290" s="5" t="b">
         <v>0</v>
@@ -14357,24 +14330,24 @@
         <v>1</v>
       </c>
       <c r="L290" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M290" s="23" t="s">
         <v>694</v>
       </c>
       <c r="N290" s="5" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="291" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A291" s="5" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B291" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C291" s="5" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="D291" s="28" t="s">
         <v>738</v>
@@ -14383,7 +14356,7 @@
         <v>350</v>
       </c>
       <c r="H291" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I291" s="5" t="b">
         <v>0</v>
@@ -14393,24 +14366,24 @@
         <v>1</v>
       </c>
       <c r="L291" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M291" s="23" t="s">
         <v>691</v>
       </c>
       <c r="N291" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="292" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A292" s="5" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="B292" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C292" s="5" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="D292" s="28" t="s">
         <v>738</v>
@@ -14419,7 +14392,7 @@
         <v>350</v>
       </c>
       <c r="H292" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I292" s="5" t="b">
         <v>0</v>
@@ -14429,24 +14402,24 @@
         <v>1</v>
       </c>
       <c r="L292" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M292" s="23" t="s">
         <v>690</v>
       </c>
       <c r="N292" s="5" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="293" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A293" s="5" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B293" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C293" s="5" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D293" s="28" t="s">
         <v>738</v>
@@ -14455,7 +14428,7 @@
         <v>350</v>
       </c>
       <c r="H293" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I293" s="5" t="b">
         <v>0</v>
@@ -14465,24 +14438,24 @@
         <v>1</v>
       </c>
       <c r="L293" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M293" s="23" t="s">
         <v>693</v>
       </c>
       <c r="N293" s="5" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="294" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A294" s="5" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B294" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C294" s="5" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D294" s="28" t="s">
         <v>738</v>
@@ -14491,7 +14464,7 @@
         <v>350</v>
       </c>
       <c r="H294" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I294" s="5" t="b">
         <v>0</v>
@@ -14501,24 +14474,24 @@
         <v>1</v>
       </c>
       <c r="L294" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M294" s="23" t="s">
         <v>694</v>
       </c>
       <c r="N294" s="5" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="295" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A295" s="5" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B295" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C295" s="5" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="D295" s="28" t="s">
         <v>738</v>
@@ -14527,7 +14500,7 @@
         <v>350</v>
       </c>
       <c r="H295" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I295" s="5" t="b">
         <v>0</v>
@@ -14537,24 +14510,24 @@
         <v>1</v>
       </c>
       <c r="L295" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M295" s="23" t="s">
         <v>691</v>
       </c>
       <c r="N295" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="296" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A296" s="5" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B296" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C296" s="5" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D296" s="28" t="s">
         <v>738</v>
@@ -14563,7 +14536,7 @@
         <v>350</v>
       </c>
       <c r="H296" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I296" s="5" t="b">
         <v>0</v>
@@ -14573,24 +14546,24 @@
         <v>1</v>
       </c>
       <c r="L296" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M296" s="23" t="s">
         <v>690</v>
       </c>
       <c r="N296" s="5" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="297" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A297" s="5" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B297" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C297" s="5" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D297" s="28" t="s">
         <v>738</v>
@@ -14599,7 +14572,7 @@
         <v>350</v>
       </c>
       <c r="H297" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I297" s="5" t="b">
         <v>0</v>
@@ -14609,24 +14582,24 @@
         <v>1</v>
       </c>
       <c r="L297" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M297" s="23" t="s">
         <v>691</v>
       </c>
       <c r="N297" s="5" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="298" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A298" s="5" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B298" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C298" s="5" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D298" s="28" t="s">
         <v>738</v>
@@ -14635,7 +14608,7 @@
         <v>350</v>
       </c>
       <c r="H298" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I298" s="5" t="b">
         <v>0</v>
@@ -14645,24 +14618,24 @@
         <v>1</v>
       </c>
       <c r="L298" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M298" s="23" t="s">
         <v>690</v>
       </c>
       <c r="N298" s="5" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="299" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A299" s="5" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B299" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C299" s="5" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D299" s="28" t="s">
         <v>738</v>
@@ -14671,7 +14644,7 @@
         <v>350</v>
       </c>
       <c r="H299" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I299" s="5" t="b">
         <v>0</v>
@@ -14681,24 +14654,24 @@
         <v>1</v>
       </c>
       <c r="L299" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M299" s="23" t="s">
         <v>693</v>
       </c>
       <c r="N299" s="5" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="300" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A300" s="5" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B300" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D300" s="28" t="s">
         <v>738</v>
@@ -14707,7 +14680,7 @@
         <v>350</v>
       </c>
       <c r="H300" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I300" s="5" t="b">
         <v>0</v>
@@ -14717,24 +14690,24 @@
         <v>1</v>
       </c>
       <c r="L300" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M300" s="23" t="s">
         <v>694</v>
       </c>
       <c r="N300" s="5" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="301" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A301" s="5" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B301" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C301" s="5" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D301" s="28" t="s">
         <v>738</v>
@@ -14743,7 +14716,7 @@
         <v>350</v>
       </c>
       <c r="H301" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I301" s="5" t="b">
         <v>0</v>
@@ -14753,24 +14726,24 @@
         <v>1</v>
       </c>
       <c r="L301" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M301" s="23" t="s">
         <v>691</v>
       </c>
       <c r="N301" s="5" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="302" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A302" s="5" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B302" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C302" s="5" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="D302" s="28" t="s">
         <v>738</v>
@@ -14779,7 +14752,7 @@
         <v>350</v>
       </c>
       <c r="H302" s="5" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I302" s="5" t="b">
         <v>0</v>
@@ -14789,24 +14762,24 @@
         <v>1</v>
       </c>
       <c r="L302" s="23" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M302" s="23" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="N302" s="5" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="303" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A303" s="5" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="B303" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C303" s="5" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D303" s="28" t="s">
         <v>738</v>
@@ -14815,7 +14788,7 @@
         <v>350</v>
       </c>
       <c r="H303" s="5" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="I303" s="5" t="b">
         <v>0</v>
@@ -14835,22 +14808,22 @@
     </row>
     <row r="304" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A304" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="B304" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C304" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="D304" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="E304" s="23" t="s">
+        <v>350</v>
+      </c>
+      <c r="H304" s="5" t="s">
         <v>835</v>
-      </c>
-      <c r="B304" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C304" s="5" t="s">
-        <v>836</v>
-      </c>
-      <c r="D304" s="28" t="s">
-        <v>832</v>
-      </c>
-      <c r="E304" s="23" t="s">
-        <v>350</v>
-      </c>
-      <c r="H304" s="5" t="s">
-        <v>837</v>
       </c>
       <c r="I304" s="5" t="b">
         <v>0</v>
@@ -14863,10 +14836,10 @@
         <v>424</v>
       </c>
       <c r="M304" s="23" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="N304" s="5" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SB BIS Order Balance v1.0; TICC-383
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.2.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philip/dev/git-peppol/edec-codelists/work-in-progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C550A4C-B780-3541-8C30-4800C5EBCF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0386FA-0264-E344-86E3-A692AD0581F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2675" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2684" uniqueCount="844">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2634,6 +2634,21 @@
     <t>TICC-328
 TICC-374
 TICC-386</t>
+  </si>
+  <si>
+    <t>TICC-383</t>
+  </si>
+  <si>
+    <t>Order Balance</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:imda.gov.sg:bis:order_balance:1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Order-2::Order##urn:fdc:imda.gov.sg:trns:order_balance:1::2.1</t>
+  </si>
+  <si>
+    <t>SG BIS Order Balance v1.0</t>
   </si>
 </sst>
 </file>
@@ -3297,11 +3312,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N304"/>
+  <dimension ref="A1:N305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A243" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A250" sqref="A250:A253"/>
+      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A305" sqref="A305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14842,6 +14857,41 @@
         <v>837</v>
       </c>
     </row>
+    <row r="305" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A305" s="5" t="s">
+        <v>843</v>
+      </c>
+      <c r="B305" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C305" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="D305" s="28" t="s">
+        <v>830</v>
+      </c>
+      <c r="E305" s="23" t="s">
+        <v>350</v>
+      </c>
+      <c r="H305" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="I305" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J305" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L305" s="23" t="s">
+        <v>578</v>
+      </c>
+      <c r="M305" s="23" t="s">
+        <v>840</v>
+      </c>
+      <c r="N305" s="5" t="s">
+        <v>841</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N283" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>